<commit_message>
Co-authored-by: Natalin De Oliveira Santos Junior <93950955+JuniorNatalin@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/KJLTVX/Status_Robo.xlsx
+++ b/KJLTVX/Status_Robo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\junio\Desktop\Nova pasta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\junio\Documents\GitHub\VASC\KJLTVX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A12AFEA-4FDC-441F-A240-D089C6441FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD8693D-72AB-4AF6-9BF3-45400AEE90E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="643" firstSheet="1" activeTab="4" xr2:uid="{0C1DAE24-9B55-4BD7-B91B-81DE79BE140C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="643" firstSheet="1" activeTab="3" xr2:uid="{0C1DAE24-9B55-4BD7-B91B-81DE79BE140C}"/>
   </bookViews>
   <sheets>
     <sheet name="VASC LTVR" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="82">
   <si>
     <t>1120R01</t>
   </si>
@@ -1731,7 +1731,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView zoomScale="74" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -2195,8 +2195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1A96693-D7AB-452A-9BD0-CDB963ECFEE0}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="A15" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2856,9 +2856,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69781F33-9E6B-4734-B4C4-5473A1EC001A}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView zoomScale="74" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2912,7 +2912,9 @@
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
@@ -2924,7 +2926,9 @@
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
@@ -2936,7 +2940,9 @@
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="3"/>
@@ -2948,7 +2954,9 @@
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="3"/>
@@ -2960,7 +2968,9 @@
       <c r="B7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="3"/>
@@ -2973,7 +2983,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2987,7 +2997,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -3001,7 +3011,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -3015,7 +3025,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -3028,9 +3038,7 @@
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="3"/>
@@ -3164,8 +3172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{198C43F8-B65B-4687-93F5-7F1509493D86}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="74" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>